<commit_message>
Changes for setup process
</commit_message>
<xml_diff>
--- a/環境変数設定内容.xlsx
+++ b/環境変数設定内容.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Tech\FAQ\NewKB\各種資料\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsato\git\isjfaq\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -65,9 +65,6 @@
     <t>/usr/FAQsetup/</t>
   </si>
   <si>
-    <t>FAQRefOnly.xml</t>
-  </si>
-  <si>
     <t>TopicD.xml</t>
   </si>
   <si>
@@ -84,9 +81,6 @@
   </si>
   <si>
     <t>P:\Public\Tech\FAQ\NewKB\FAQsetup</t>
-  </si>
-  <si>
-    <t>FAQAllFunc.xml</t>
   </si>
   <si>
     <t>/intersystems/cache/csp/user</t>
@@ -148,14 +142,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>セットアップ用クラスxml
-(classfilename)</t>
-    <rPh sb="6" eb="7">
-      <t>ヨウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>セットアップ用グローバルxml
 (globalfilename)</t>
     <rPh sb="6" eb="7">
@@ -167,11 +153,27 @@
     <t>Knowledge</t>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>セットアップ用クラスディレクトリ
+(classfiledir)</t>
+    <rPh sb="6" eb="7">
+      <t>ヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>FAQ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>FAQ</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -546,7 +548,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
@@ -569,23 +573,23 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B3" s="4">
         <v>64</v>
@@ -597,102 +601,102 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="5" customFormat="1" ht="27" x14ac:dyDescent="0.15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="5" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="5" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="5" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="4" t="s">
+      <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" s="5" customFormat="1" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="A10" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>10</v>
-      </c>
       <c r="D10" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>